<commit_message>
Filter to sheets by item
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -1,29 +1,79 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VU\2_kursas\2_semestras\VPR\Projektinis\HubaBuba\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EAFD0AA-6B61-40DF-95DC-7B02526A6893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="4980" yWindow="2784" windowWidth="23016" windowHeight="12156" xr2:uid="{55EEE1A2-ED87-44A1-AF24-4B6D7DD2C7C0}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Iphone 11" sheetId="3" r:id="rId1"/>
+    <sheet name="usb atmintine 32gb" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>LinkToItem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.95
+</t>
+  </si>
+  <si>
+    <t>https://www.varle.lt/usb-laikmenos/atmintukas-transcend-jf500-32gb-istraukiamas--1202909.html</t>
+  </si>
+  <si>
+    <t>519</t>
+  </si>
+  <si>
+    <t>https://www.varle.lt/mobilieji-telefonai/apple-iphone-11-64gb-black--14844674.html</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -49,13 +99,212 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -66,6 +315,28 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{BC7EB4AA-D7C7-47B2-975C-EB15167D65F3}" name="Table2" displayName="Table2" ref="A1:B2" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
+  <autoFilter ref="A1:B2" xr:uid="{BC7EB4AA-D7C7-47B2-975C-EB15167D65F3}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{20BF7205-C4C0-4F72-9FB3-39030E33B374}" name="Price" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{D189B7FE-9889-4237-9305-0C6A95D15E42}" name="LinkToItem" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{613AA139-8E22-4C68-ACEC-03267AE9FEF9}" name="Table1" displayName="Table1" ref="A1:B2" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:B2" xr:uid="{613AA139-8E22-4C68-ACEC-03267AE9FEF9}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{078C23D2-64E9-4908-9A18-40E079E1D649}" name="Price" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{F07F8D57-C174-46A5-A374-B0C788F5C927}" name="LinkToItem" dataDxfId="4"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -85,7 +356,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -97,7 +368,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -144,6 +415,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -179,6 +467,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -330,12 +635,87 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A726A9C4-F3E5-436C-AF5F-8BFB03CB96CD}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CDC3EAC-D23F-4860-9600-83AD0C90E335}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="83.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{561BBAF5-216B-42F3-8E84-EF8F2903D3CB}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added new shop topo centras
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kazen\Documents\UiPath\Robotas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24572FFA-66EE-498D-B6B0-EA01D7BE47A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54A7B6DB-2507-47CA-A69F-7DCA55AC6F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-11355" yWindow="315" windowWidth="8775" windowHeight="11745" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>Price</t>
   </si>
@@ -65,6 +65,12 @@
   </si>
   <si>
     <t>https://www.skytech.lt/mwhh2eta-iphone-pro-max-64gb-midnight-green-p-469291.html</t>
+  </si>
+  <si>
+    <t>529,,00</t>
+  </si>
+  <si>
+    <t>https://www.topocentras.lt/mobilusis-telefonas-apple-iphone-11-64gb-black.html</t>
   </si>
 </sst>
 </file>
@@ -323,22 +329,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9A11961B-15DF-4769-8215-0298F434E516}" name="Table2" displayName="Table2" ref="A1:B3" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
-  <autoFilter ref="A1:B3" xr:uid="{9A11961B-15DF-4769-8215-0298F434E516}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5EA0D5FD-1EB8-4D2D-A081-A2CAFCC3AF0B}" name="Table2" displayName="Table2" ref="A1:B4" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
+  <autoFilter ref="A1:B4" xr:uid="{5EA0D5FD-1EB8-4D2D-A081-A2CAFCC3AF0B}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{D4D540E6-2E07-4514-8717-B0E952CE889A}" name="Price" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{12645396-88A1-48D1-A7B8-97F25C0D389F}" name="LinkToItem" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{AC482D72-D3D0-47FD-9B2E-7512A0FE690F}" name="Price" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{FC4EFB22-F0F1-4A43-AEE9-FDFE7D131F6A}" name="LinkToItem" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8D2A33D2-879B-47F2-9EB7-BEF57245712E}" name="Table1" displayName="Table1" ref="A1:B3" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:B3" xr:uid="{8D2A33D2-879B-47F2-9EB7-BEF57245712E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4FDD67C5-81BA-4CE0-A8CE-9D689BF19039}" name="Table1" displayName="Table1" ref="A1:B4" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:B4" xr:uid="{4FDD67C5-81BA-4CE0-A8CE-9D689BF19039}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{D93CA3AF-0D49-4464-8C12-DD3C26D94201}" name="Price" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{84FA8D45-D9CC-4F3E-9F3A-A452BF478450}" name="LinkToItem" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{167E763E-261E-4FD4-8B92-19DE35451B36}" name="Price" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{F8DEC9B9-862C-4F6C-AD7B-B0152F85679C}" name="LinkToItem" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -640,8 +646,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BE84F47-5925-4F00-B647-A6B47D8EC89C}">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AA152E6-4218-45B8-BDCD-459EF3D47124}">
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -676,6 +682,14 @@
         <v>8</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -685,8 +699,8 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4F334FA-0B2A-469C-BB10-7D5C9FA35826}">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C861056-4574-4CDB-8F1C-AD054598335F}">
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -721,11 +735,18 @@
         <v>4</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Changes in skytech search
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kazen\Documents\UiPath\Robotas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54A7B6DB-2507-47CA-A69F-7DCA55AC6F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{444DBE2C-F860-4E75-9F38-CF612390E5CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-11355" yWindow="315" windowWidth="8775" windowHeight="11745" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Iphone 11" sheetId="3" r:id="rId1"/>
-    <sheet name="usb atmintine 32gb" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Jbl go" sheetId="4" r:id="rId1"/>
+    <sheet name="Iphone 11" sheetId="3" r:id="rId2"/>
+    <sheet name="usb atmintine 32gb" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>Price</t>
   </si>
@@ -61,16 +62,34 @@
     <t>https://www.varle.lt/mobilieji-telefonai/apple-iphone-11-64gb-black--14844674.html</t>
   </si>
   <si>
-    <t>768.,00</t>
-  </si>
-  <si>
-    <t>https://www.skytech.lt/mwhh2eta-iphone-pro-max-64gb-midnight-green-p-469291.html</t>
+    <t>524.,00</t>
+  </si>
+  <si>
+    <t>https://www.skytech.lt/mhda3eta-apple-iphone-64gb-juodas-ismanusis-telefonas-p-531837.html</t>
   </si>
   <si>
     <t>529,,00</t>
   </si>
   <si>
     <t>https://www.topocentras.lt/mobilusis-telefonas-apple-iphone-11-64gb-black.html</t>
+  </si>
+  <si>
+    <t>43.91</t>
+  </si>
+  <si>
+    <t>https://www.varle.lt/nesiojamos-mobilios-koloneles/nesiojama-kolonele-jbl-go-3-bt-tamsiai-melyna--14843834.html</t>
+  </si>
+  <si>
+    <t>49.,19</t>
+  </si>
+  <si>
+    <t>https://www.skytech.lt/jblgo3grn-jbl-zalia-beviele-mobili-bluetooth-kolonele-vandeniui-smugiams-atspari-p-531726.html</t>
+  </si>
+  <si>
+    <t>Su TOPO KLUBU jus sutaupote 1,,00</t>
+  </si>
+  <si>
+    <t>https://www.topocentras.lt/nesiojamas-garsiakalbis-jbl-go-3-ipx7-juodas.html</t>
   </si>
 </sst>
 </file>
@@ -122,7 +141,103 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -329,22 +444,33 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5EA0D5FD-1EB8-4D2D-A081-A2CAFCC3AF0B}" name="Table2" displayName="Table2" ref="A1:B4" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
-  <autoFilter ref="A1:B4" xr:uid="{5EA0D5FD-1EB8-4D2D-A081-A2CAFCC3AF0B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{EFB322DF-F7A4-47C2-B60F-35B98A0F5F0E}" name="Table3" displayName="Table3" ref="A1:B4" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
+  <autoFilter ref="A1:B4" xr:uid="{EFB322DF-F7A4-47C2-B60F-35B98A0F5F0E}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{AC482D72-D3D0-47FD-9B2E-7512A0FE690F}" name="Price" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{FC4EFB22-F0F1-4A43-AEE9-FDFE7D131F6A}" name="LinkToItem" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{6DF052BB-F862-45D2-A24F-A0F7D31EBDA2}" name="Price" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{D855FA3B-D848-414F-86C7-F30583225F57}" name="LinkToItem" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4FDD67C5-81BA-4CE0-A8CE-9D689BF19039}" name="Table1" displayName="Table1" ref="A1:B4" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:B4" xr:uid="{4FDD67C5-81BA-4CE0-A8CE-9D689BF19039}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AC039BA3-EE3C-4DBB-84C9-FA8C24E5895E}" name="Table2" displayName="Table2" ref="A1:B4" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:B4" xr:uid="{AC039BA3-EE3C-4DBB-84C9-FA8C24E5895E}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{167E763E-261E-4FD4-8B92-19DE35451B36}" name="Price" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{F8DEC9B9-862C-4F6C-AD7B-B0152F85679C}" name="LinkToItem" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{F55E69BD-1E6B-4935-A586-07530F4EF909}" name="Price" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{F1B6884A-2C39-48A6-BA22-B0C799BF95EA}" name="LinkToItem" dataDxfId="4"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{346EA4F7-EF7E-4AA7-9F33-72D9AEBC4E1C}" name="Table1" displayName="Table1" ref="A1:B4" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A1:B4" xr:uid="{346EA4F7-EF7E-4AA7-9F33-72D9AEBC4E1C}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{C567E7AB-8A2C-47B3-8281-764F042BF801}" name="Price" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{BFA301EE-F85C-4C12-B750-124A641A08F1}" name="LinkToItem" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -646,15 +772,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AA152E6-4218-45B8-BDCD-459EF3D47124}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A243174-2140-4390-B944-52C4F3384E7C}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="113.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -668,26 +794,26 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -699,7 +825,60 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C861056-4574-4CDB-8F1C-AD054598335F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79960BEE-5598-4BED-8AE7-0B9161431F85}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="90.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9521B92C-5EEE-4C52-AF1E-FA2312901394}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -751,7 +930,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>